<commit_message>
Impresion Lista Oficial Part1 EXCEL
</commit_message>
<xml_diff>
--- a/app/reportes/reporte.xlsx
+++ b/app/reportes/reporte.xlsx
@@ -15,30 +15,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>NO CUENTA</t>
-  </si>
-  <si>
-    <t>PRIMER APELLIDO</t>
-  </si>
-  <si>
-    <t>SEGUNDO APELLIDO</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>CORREO</t>
-  </si>
-  <si>
-    <t>TELEFONO</t>
-  </si>
-  <si>
-    <t>CARRERA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+  <si>
+    <t>Lista Oficial</t>
+  </si>
+  <si>
+    <t>SICEP - Centro de Computo</t>
+  </si>
+  <si>
+    <t>PROFESOR:</t>
+  </si>
+  <si>
+    <t>Christian RCGS DEVELOPER</t>
+  </si>
+  <si>
+    <t>No TRABAJADOR:</t>
+  </si>
+  <si>
+    <t>SEMINARIO</t>
+  </si>
+  <si>
+    <t>003 Aspel COI</t>
+  </si>
+  <si>
+    <t>GRUPO:</t>
+  </si>
+  <si>
+    <t>SEMESTRE:</t>
+  </si>
+  <si>
+    <t>2021-2</t>
+  </si>
+  <si>
+    <t>GENERACION:</t>
+  </si>
+  <si>
+    <t>MODALIDAD:</t>
+  </si>
+  <si>
+    <t>Presencial</t>
+  </si>
+  <si>
+    <t>Abasolo</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>juan@algo.com</t>
+  </si>
+  <si>
+    <t>5512457845</t>
+  </si>
+  <si>
+    <t>Ing. en Alimentos</t>
   </si>
   <si>
     <t>Hernandez</t>
@@ -64,13 +97,49 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -92,8 +161,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -395,68 +476,133 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="1">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D5" s="4">
+        <v>312260633</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
+      <c r="C7" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2022</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B10">
+        <v>55555555</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
         <v>456156165</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>